<commit_message>
Consolidation of Data Layer
</commit_message>
<xml_diff>
--- a/John.SocialClub/MosqueCommunity.Data/DatabaseLogic/Communnity.xlsx
+++ b/John.SocialClub/MosqueCommunity.Data/DatabaseLogic/Communnity.xlsx
@@ -24,9 +24,6 @@
     <t>TEACHER</t>
   </si>
   <si>
-    <t>LESSON</t>
-  </si>
-  <si>
     <t>PREMISES</t>
   </si>
   <si>
@@ -36,9 +33,6 @@
     <t>SCHEDULE (Lesson, Premise, Teacher,Time)</t>
   </si>
   <si>
-    <t>ClassHOURS</t>
-  </si>
-  <si>
     <t>ENTITIES</t>
   </si>
   <si>
@@ -52,6 +46,12 @@
   </si>
   <si>
     <t>TEST (List of Student,Lesson</t>
+  </si>
+  <si>
+    <t>SUBJECTS</t>
+  </si>
+  <si>
+    <t>CALENDAR</t>
   </si>
 </sst>
 </file>
@@ -433,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C4:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -447,21 +447,21 @@
   <sheetData>
     <row r="4" spans="3:6">
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="F4" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="3:6">
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -471,7 +471,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E6" s="4"/>
     </row>
@@ -484,23 +484,23 @@
     </row>
     <row r="8" spans="3:6" ht="30" customHeight="1">
       <c r="C8" s="5" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="3:6" ht="36.6" customHeight="1">
       <c r="C9" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="3:6" ht="33" customHeight="1">
       <c r="C10" s="5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>

</xml_diff>